<commit_message>
updated code of 02-05-25
</commit_message>
<xml_diff>
--- a/client/public/sample_leads.xlsx
+++ b/client/public/sample_leads.xlsx
@@ -16,9 +16,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t>Lead Number</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -32,13 +29,16 @@
   </si>
   <si>
     <t>Actual Date</t>
+  </si>
+  <si>
+    <t>Email Id</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -50,6 +50,14 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -75,10 +83,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -418,11 +427,12 @@
   <dimension ref="A1:V8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="8.75" customWidth="1"/>
     <col min="6" max="7" width="10.125" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="10.125" bestFit="1" customWidth="1"/>
     <col min="21" max="24" width="10.125" bestFit="1" customWidth="1"/>
@@ -441,11 +451,11 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">

</xml_diff>